<commit_message>
added img folder and minor changes
</commit_message>
<xml_diff>
--- a/src/sample.xlsx
+++ b/src/sample.xlsx
@@ -1,59 +1,59 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet state="visible" name="Pre program run" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Post program run" sheetId="2" r:id="rId5"/>
+    <sheet sheetId="1" name="Pre program run" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Post program run" state="visible" r:id="rId5"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
   <si>
     <t>Website</t>
   </si>
   <si>
+    <t>Category</t>
+  </si>
+  <si>
     <t>https://www.headphonezone.in/</t>
   </si>
   <si>
+    <t>SHOPIFY</t>
+  </si>
+  <si>
     <t>https://www.boat-lifestyle.com/</t>
   </si>
   <si>
     <t>somemadeupwebsite.com</t>
   </si>
   <si>
+    <t>NOT_WORKING</t>
+  </si>
+  <si>
     <t>https://nutrabay.com/</t>
   </si>
   <si>
+    <t>WOOCOMMERCE</t>
+  </si>
+  <si>
     <t>https://shop.waaree.com/</t>
   </si>
   <si>
+    <t>BIGCOMMERCE</t>
+  </si>
+  <si>
     <t>https://www.cult.fit/store/gear</t>
   </si>
   <si>
+    <t>OTHERS</t>
+  </si>
+  <si>
     <t>https://www.ritukumar.com/</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>SHOPIFY</t>
-  </si>
-  <si>
-    <t>NOT_WORKING</t>
-  </si>
-  <si>
-    <t>WOOCOMMERCE</t>
-  </si>
-  <si>
-    <t>BIGCOMMERCE</t>
-  </si>
-  <si>
-    <t>OTHERS</t>
   </si>
   <si>
     <t>MAGENTO</t>
@@ -62,36 +62,50 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
-    <font>
-      <sz val="10.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8" x14ac:knownFonts="1">
+    <font>
+      <color theme="1"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <scheme val="minor"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF1155CC"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <sz val="10"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <scheme val="minor"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color rgb="FF000000"/>
+      <scheme val="minor"/>
+      <sz val="10"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10.0"/>
-      <color rgb="FF1155CC"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10.0"/>
-      <color rgb="FF0000FF"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,48 +113,55 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -338,161 +359,185 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" defaultColWidth="12.63" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="24.13"/>
-    <col customWidth="1" min="2" max="2" width="15.13"/>
+    <col min="1" max="1" width="24.13" customWidth="1"/>
+    <col min="2" max="2" width="15.13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2"/>
-    <hyperlink r:id="rId2" ref="A3"/>
-    <hyperlink r:id="rId3" ref="A4"/>
-    <hyperlink r:id="rId4" ref="A5"/>
-    <hyperlink r:id="rId5" ref="A6"/>
-    <hyperlink r:id="rId6" ref="A7"/>
-    <hyperlink r:id="rId7" ref="A8"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
   </hyperlinks>
-  <drawing r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" defaultColWidth="12.63" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="24.13"/>
-    <col customWidth="1" min="2" max="2" width="15.13"/>
+    <col min="1" max="1" width="24.13" customWidth="1"/>
+    <col min="2" max="2" width="15.13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2"/>
-    <hyperlink r:id="rId2" ref="A3"/>
-    <hyperlink r:id="rId3" ref="A4"/>
-    <hyperlink r:id="rId4" ref="A5"/>
-    <hyperlink r:id="rId5" ref="A6"/>
-    <hyperlink r:id="rId6" ref="A7"/>
-    <hyperlink r:id="rId7" ref="A8"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
   </hyperlinks>
-  <drawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>